<commit_message>
Updated tasks to use scanner key 5
</commit_message>
<xml_diff>
--- a/fingersBlock.xlsx
+++ b/fingersBlock.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lydia\Documents\Code\PsychoPy\fMRI block tasks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lydia\Documents\Code\PsychoPy\fMRI_Block_Tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8742C1-59B6-4AF4-AB95-A4B115506841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E55946-7A90-4CFD-AB3C-5E8F36995B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="38560" windowHeight="21040" xr2:uid="{F303154F-1C1F-4DF0-A8A4-DF89E4337BE6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{F303154F-1C1F-4DF0-A8A4-DF89E4337BE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -528,45 +528,45 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7265625" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7265625" style="2"/>
+    <col min="1" max="1" width="20.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>

</xml_diff>